<commit_message>
delete & add in stock page
1. basically finish the add and delete function on stock page
2. fix the child and parent window problem
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Associated Technology</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>blockchain</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
keyword page update: add and delete
add and delete done
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -722,16 +722,18 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>btc</t>
+          <t>ftm</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>12</v>
+          <t>Associated Technology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>blockchain</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -747,11 +749,13 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>13</v>
+          <t>Significant Persons</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>elon musk</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -762,7 +766,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>btc</t>
+          <t>eth</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -770,8 +774,10 @@
           <t>Significant Related Persons</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>14</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Vitalik Buterin</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -790,8 +796,10 @@
           <t>Significant Related Persons</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>15</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vip1</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -810,8 +818,10 @@
           <t>Significant Related Persons</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>16</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>vip2</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -830,8 +840,10 @@
           <t>Significant Related Persons</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>17</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>vip3</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -847,11 +859,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>18</v>
+          <t>Associated Technology</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>tech1</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -862,7 +876,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ftm</t>
+          <t>btc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -872,7 +886,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>blockchain</t>
+          <t>tech2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -884,17 +898,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Luna</t>
+          <t>btc</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Correlated Concept</t>
+          <t>Associated Technology</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>btc</t>
+          <t>tech3</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -911,37 +925,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Significant Persons</t>
+          <t>Correlated Concept</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>elon musk</t>
+          <t>concept1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
-        <is>
-          <t>test111</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>eth</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Significant Related Persons</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Vitalik Buterin</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
         <is>
           <t>test111</t>
         </is>

</xml_diff>

<commit_message>
function on Person page
not finished yet
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,7 +766,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>eth</t>
+          <t>btc</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vitalik Buterin</t>
+          <t>vip1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>vip1</t>
+          <t>vip2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>vip2</t>
+          <t>vip3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -837,12 +837,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
+          <t>Associated Technology</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>vip3</t>
+          <t>tech1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -864,7 +864,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>tech1</t>
+          <t>tech2</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>tech2</t>
+          <t>tech3</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -903,12 +903,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Associated Technology</t>
+          <t>Correlated Concept</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>tech3</t>
+          <t>concept1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -920,20 +920,108 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>btc</t>
+          <t>eth</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Correlated Concept</t>
+          <t>Significant Related Persons</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>concept1</t>
+          <t>VitalikButerin</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Significant Related Persons</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ethereum</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Significant Related Persons</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>brian_armstrong</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Significant Related Persons</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CoinDesk</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Significant Related Persons</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>vip1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
         <is>
           <t>test111</t>
         </is>

</xml_diff>

<commit_message>
concept page update and test
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,6 +1159,50 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Correlated Concept</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ETC</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Correlated Concept</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>DeFi</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
event page update and test
basically finish the whole skeleton of the app, what remains to be done is to apply some adaptive adjustment (functions) to different page
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,6 +1203,28 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Influential Event</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>merge</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
remark function add to the keyword page
</commit_message>
<xml_diff>
--- a/v 2.0/tweetsa_user_data.xlsx
+++ b/v 2.0/tweetsa_user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -934,7 +934,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VitalikButerin</t>
+          <t>brian_armstrong</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>brian_armstrong</t>
+          <t>CoinDesk</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CoinDesk</t>
+          <t>CryptosisAI</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -998,12 +998,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
+          <t>Associated Technology</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CryptosisAI</t>
+          <t>Serenity</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>smart contracts</t>
+          <t>Casper</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Serenity</t>
+          <t>VDF</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Casper</t>
+          <t>Beacon chain</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VDF</t>
+          <t>ERC</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1113,12 +1113,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Associated Technology</t>
+          <t>Significant Related Persons</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Beacon chain</t>
+          <t>ForbesCrypto</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1136,12 +1136,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Associated Technology</t>
+          <t>Influential Event</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ERC</t>
+          <t>merge</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1159,12 +1159,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Significant Related Persons</t>
+          <t>Associated Technology</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ForbesCrypto</t>
+          <t>blockchain</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1172,7 +1172,11 @@
           <t>test111</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>The core technology of Ethereum</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1182,12 +1186,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Correlated Concept</t>
+          <t>Significant Related Persons</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ETC</t>
+          <t>VitalikButerin</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1195,7 +1199,11 @@
           <t>test111</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Russian-born Canadian programmer and writer who is best known as one of the co-founders of Ethereum</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1205,12 +1213,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Correlated Concept</t>
+          <t>Associated Technology</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>DeFi</t>
+          <t>smart contracts</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1218,7 +1226,11 @@
           <t>test111</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>A smart contract, like any contract, establishes the terms of an agreement. But unlike a traditional contract, a smart contract’s terms are executed as code running on a blockchain like Ethereum. Smart contracts allow developers to build apps that take advantage of blockchain security, reliability, and accessibility while offering sophisticated peer-to-peer functionality — everything from loans and insurance to logistics and gaming.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1228,12 +1240,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Influential Event</t>
+          <t>Correlated Concept</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>merge</t>
+          <t>ETC</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1241,7 +1253,11 @@
           <t>test111</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>ETC is the native cryptocurrency of Ethereum Classic, a blockchain project that was created in 2016 when Ethereum’s blockchain split into two separate chains following a disagreement among members of its community.</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1251,12 +1267,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Associated Technology</t>
+          <t>Correlated Concept</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>blockchain</t>
+          <t>DeFi</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1266,7 +1282,37 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>The core technology of Ethereum</t>
+          <t>Decentralized finance (DeFi) is an emerging financial technology based on secure distributed ledgers similar to those used by cryptocurrencies. The system removes the control banks and institutions have on money, financial products, and financial services.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Correlated Concept</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>merge</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>test111</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Eventually the current Ethereum Mainnet will "merge" with the beacon chain proof-of-stake system.
+This will mark the end of proof-of-work for Ethereum, and the full transition to proof-of-stake.
+This is planned to precede the roll out of shard chains.
+We formerly referred to this as "the docking."</t>
         </is>
       </c>
     </row>

</xml_diff>